<commit_message>
Merge Docs and Sim
</commit_message>
<xml_diff>
--- a/TESS_Docs/calculator.xlsx
+++ b/TESS_Docs/calculator.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Things\EPAE\Microcontrolere\Arduino\Arduino_sketches\TESS\TESS_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\casdev\sbxs\github.conti.de\TESS\TESS_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD41DCB-D4FE-402D-906F-5EE6A8ED4110}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="744" firstSheet="2" activeTab="7"/>
+    <workbookView minimized="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" tabRatio="744" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mot_Param" sheetId="4" r:id="rId1"/>
@@ -20,23 +21,30 @@
     <sheet name="bemf_Kt" sheetId="3" r:id="rId6"/>
     <sheet name="SpeedSensorOpAmpG&amp;O" sheetId="8" r:id="rId7"/>
     <sheet name="CurrentSensingOpAmpGain" sheetId="9" r:id="rId8"/>
+    <sheet name="TImers" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>AA</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>clock_f</t>
   </si>
@@ -367,11 +375,34 @@
   <si>
     <t>Rin</t>
   </si>
+  <si>
+    <t>Desired interrupt period</t>
+  </si>
+  <si>
+    <t>Tcnt</t>
+  </si>
+  <si>
+    <t>Tarr</t>
+  </si>
+  <si>
+    <t>SysClk</t>
+  </si>
+  <si>
+    <t>Tpsc</t>
+  </si>
+  <si>
+    <t>Actual Period</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="172" formatCode="0.0000000000"/>
+    <numFmt numFmtId="174" formatCode="0.000000000000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,12 +488,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,6 +512,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +552,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -561,7 +601,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -849,7 +895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -948,10 +994,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1082,7 +1128,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1192,7 +1238,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1268,7 +1314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1308,7 +1354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1407,7 +1453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1539,7 +1585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -1553,259 +1599,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>4.82</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>2.5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.17</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <f>(B3-B4)/(B5-B6)</f>
         <v>13.647058823529413</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <f>B4-(B8*B6)</f>
         <v>2.5</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>1720</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <f>B2*B11*B8/B9</f>
         <v>46945.882352941182</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>1330</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <f>B12*B13/(B8*(B11+B12)-B12)</f>
         <v>101.16331096196868</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,10 +1861,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1829,223 +1875,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>4.82</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.81</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <f>(B3)/(B5)</f>
         <v>5.9506172839506171</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>180</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <f>(B8-1)*B10</f>
         <v>891.11111111111109</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987934E8-AF84-4E17-B244-6C0CEE42590C}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="14">
+        <f>B6*B5</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>84000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>((B1*B3)/B5)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>8400</v>
+      </c>
+      <c r="C5">
+        <f>B1/B6</f>
+        <v>8400</v>
+      </c>
+      <c r="E5">
+        <f>4000/0.0001</f>
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="15">
+        <f>(B4+1)/B3</f>
+        <v>1.1904761904761905E-8</v>
+      </c>
+      <c r="E6" s="16">
+        <f>B6*12</f>
+        <v>1.4285714285714287E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>